<commit_message>
add python methods to the ontology
This push has the methods that answer the comptency questions
These methods are used to evaulate the comptency questions.
</commit_message>
<xml_diff>
--- a/competency.xlsx
+++ b/competency.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/builds/ontology-build/conference paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3DB0B937-CFA0-6144-9AEA-65E899912222}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF86C7C-B1AA-E64C-95E8-98DBD87C05E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5160" yWindow="1800" windowWidth="28040" windowHeight="17440" xr2:uid="{55325ED3-C5E3-1E4D-BFE5-E80D4B20F82E}"/>
+    <workbookView xWindow="-33600" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{55325ED3-C5E3-1E4D-BFE5-E80D4B20F82E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>What is the severity level of a specific defect?</t>
   </si>
@@ -43,9 +43,6 @@
     <t>Competency Question</t>
   </si>
   <si>
-    <t>SPAQRL Query</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -68,13 +65,25 @@
   </si>
   <si>
     <t>What material is the component made of?</t>
+  </si>
+  <si>
+    <t>What material is the defect of the material located on?</t>
+  </si>
+  <si>
+    <t>what bridge component is the healthiest?</t>
+  </si>
+  <si>
+    <t>what bridge component is the compromised?</t>
+  </si>
+  <si>
+    <t>What events are most frequently associated with severe defects?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -82,16 +91,48 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -99,12 +140,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,66 +481,107 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C179CF8D-01B3-514B-BD47-ECC70ADF0D0C}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="76.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="5"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="5"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="5"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="B6" s="4"/>
+      <c r="C6" s="5"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="6"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="B8" s="4"/>
+      <c r="C8" s="5"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="B9" s="4"/>
+      <c r="C9" s="5"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="5"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="5"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="5"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B13" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>